<commit_message>
74LS373 PPU AD Pins FIX
Fixed 74LS373 pins connected to the AD Pins from PPU (PPU D0 to D7)
</commit_message>
<xml_diff>
--- a/BOM-ListaDeMateriais.xlsx
+++ b/BOM-ListaDeMateriais.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vagner\VagNES\OpenPhantom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1FAC2A-6583-469C-A41B-FB2B4E74D695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763209F5-C7F3-431C-92BD-0EEB965727E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenPhantom" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">OpenPhantom!$A$1:$C$52</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>C1</t>
   </si>
@@ -228,9 +231,6 @@
   </si>
   <si>
     <t>Resistor 1/4W 10K ohm</t>
-  </si>
-  <si>
-    <t>Resistor 1/4W</t>
   </si>
   <si>
     <t>Resistor 1/4W 150K</t>
@@ -932,6 +932,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -960,22 +976,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -991,12 +991,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A2:C52" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A2:C52" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A2:C52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Referência/Reference" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="QTD/QTY" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descrição/Description" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Referência/Reference" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="QTD/QTY" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Descrição/Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1299,39 +1299,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="74.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="74.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1339,10 +1339,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
@@ -1350,13 +1350,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1364,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -1375,10 +1375,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1386,10 +1386,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1397,10 +1397,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1408,10 +1408,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1419,10 +1419,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1430,10 +1430,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1441,10 +1441,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1452,10 +1452,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1463,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -1485,10 +1485,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1496,10 +1496,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1507,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1518,10 +1518,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -1578,11 +1578,8 @@
       <c r="J24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
@@ -1590,10 +1587,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1601,10 +1598,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
@@ -1612,10 +1609,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -1623,10 +1620,10 @@
         <v>2</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1634,10 +1631,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1645,10 +1642,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
@@ -1656,10 +1653,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>55</v>
       </c>
@@ -1667,10 +1664,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
@@ -1678,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -1689,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>56</v>
       </c>
@@ -1700,10 +1697,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>26</v>
       </c>
@@ -1711,10 +1708,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>27</v>
       </c>
@@ -1722,10 +1719,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>28</v>
       </c>
@@ -1733,10 +1730,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>29</v>
       </c>
@@ -1744,10 +1741,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>30</v>
       </c>
@@ -1755,10 +1752,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
@@ -1766,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>32</v>
       </c>
@@ -1780,7 +1777,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>33</v>
       </c>
@@ -1791,7 +1788,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
@@ -1802,7 +1799,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
@@ -1813,7 +1810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -1824,7 +1821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
@@ -1835,7 +1832,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
@@ -1846,7 +1843,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>41</v>
       </c>
@@ -1857,7 +1854,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>43</v>
       </c>
@@ -1868,7 +1865,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
@@ -1879,7 +1876,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>45</v>
       </c>
@@ -1887,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1895,7 +1892,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>